<commit_message>
Update gitignore for CleverCloud deployment
</commit_message>
<xml_diff>
--- a/stream3_visualization/Well-being/data/2025-08-29_EWBI-Renaming of Primary Indicators.xlsx
+++ b/stream3_visualization/Well-being/data/2025-08-29_EWBI-Renaming of Primary Indicators.xlsx
@@ -1,12 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20417"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\valentin.stuhlfauth\OneDrive - univ-lyon2.fr\Bureau\git-Data4Good\13_democratiser_sobriete\stream3_visualization\Well-being\data\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="2" documentId="11_E47581067EFA48855B207E265B8E6C1B01B1CEB9" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{FF718A68-91D0-445D-A6A0-B5EEA3E5E72F}"/>
+  <bookViews>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8130" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Feuil1" sheetId="1" r:id="rId4"/>
+    <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0"/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion2">
       <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataChecksum="O43jDpdjw2W0uLF4HKDuBRmnMB4S78eufQ70IGnwmis="/>
@@ -16,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="103">
   <si>
     <t>Current acronym</t>
   </si>
@@ -24,9 +33,6 @@
     <t>Current name in the DB</t>
   </si>
   <si>
-    <t xml:space="preserve">Proposed name </t>
-  </si>
-  <si>
     <t>Agriculture and Food</t>
   </si>
   <si>
@@ -322,30 +328,37 @@
   </si>
   <si>
     <t>Wanted to Learn, But Couldn't Participate</t>
+  </si>
+  <si>
+    <t>EU priority</t>
+  </si>
+  <si>
+    <t>Proposed name</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4">
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
     </font>
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Times New Roman"/>
     </font>
     <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
       <scheme val="minor"/>
@@ -356,36 +369,45 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
   </fills>
   <borders count="1">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="4">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -575,28 +597,32 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <sheetPr>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="38.63"/>
-    <col customWidth="1" min="2" max="2" width="14.5"/>
-    <col customWidth="1" min="3" max="3" width="94.25"/>
-    <col customWidth="1" min="4" max="4" width="33.13"/>
-    <col customWidth="1" min="5" max="26" width="10.63"/>
+    <col min="1" max="1" width="38.6640625" customWidth="1"/>
+    <col min="2" max="2" width="14.5" customWidth="1"/>
+    <col min="3" max="3" width="94.25" customWidth="1"/>
+    <col min="4" max="4" width="33.1640625" customWidth="1"/>
+    <col min="5" max="26" width="10.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="14.25" customHeight="1">
-      <c r="A1" s="1"/>
+    <row r="1" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A1" s="1" t="s">
+        <v>101</v>
+      </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -604,7 +630,7 @@
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>2</v>
+        <v>102</v>
       </c>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
@@ -629,438 +655,438 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" ht="14.25" customHeight="1">
+    <row r="2" spans="1:26" ht="14.25" customHeight="1">
       <c r="A2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="C2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="D2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="2" t="s">
+    </row>
+    <row r="3" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="3" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="3" ht="14.25" customHeight="1">
-      <c r="A3" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="3" t="s">
+      <c r="C3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="D3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="2" t="s">
+    </row>
+    <row r="4" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A4" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="4" ht="14.25" customHeight="1">
-      <c r="A4" s="2" t="s">
+      <c r="B4" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="C4" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="D4" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="2" t="s">
+    </row>
+    <row r="5" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A5" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="5" ht="14.25" customHeight="1">
-      <c r="A5" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B5" s="3" t="s">
+      <c r="C5" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="D5" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D5" s="2" t="s">
+    </row>
+    <row r="6" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A6" s="2" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="6" ht="14.25" customHeight="1">
-      <c r="A6" s="2" t="s">
+      <c r="B6" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="C6" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="D6" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D6" s="2" t="s">
+    </row>
+    <row r="7" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A7" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" s="3" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="7" ht="14.25" customHeight="1">
-      <c r="A7" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B7" s="3" t="s">
+      <c r="C7" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="D7" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D7" s="2" t="s">
+    </row>
+    <row r="8" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A8" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" s="3" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="8" ht="14.25" customHeight="1">
-      <c r="A8" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B8" s="3" t="s">
+      <c r="C8" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="D8" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="D8" s="2" t="s">
+    </row>
+    <row r="9" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A9" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" s="3" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="9" ht="14.25" customHeight="1">
-      <c r="A9" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B9" s="3" t="s">
+      <c r="C9" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="D9" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="D9" s="2" t="s">
+    </row>
+    <row r="10" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A10" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" s="3" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="10" ht="14.25" customHeight="1">
-      <c r="A10" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B10" s="3" t="s">
+      <c r="C10" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="D10" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="D10" s="2" t="s">
+    </row>
+    <row r="11" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A11" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11" s="3" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="11" ht="14.25" customHeight="1">
-      <c r="A11" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B11" s="3" t="s">
+      <c r="C11" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="D11" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="D11" s="2" t="s">
+    </row>
+    <row r="12" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A12" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B12" s="3" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="12" ht="14.25" customHeight="1">
-      <c r="A12" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B12" s="3" t="s">
+      <c r="C12" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="D12" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="D12" s="2" t="s">
+    </row>
+    <row r="13" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A13" s="2" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="13" ht="14.25" customHeight="1">
-      <c r="A13" s="2" t="s">
+      <c r="B13" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="C13" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="D13" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="D13" s="2" t="s">
+    </row>
+    <row r="14" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A14" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B14" s="3" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="14" ht="14.25" customHeight="1">
-      <c r="A14" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="B14" s="3" t="s">
+      <c r="C14" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="C14" s="2" t="s">
+      <c r="D14" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="D14" s="2" t="s">
+    </row>
+    <row r="15" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A15" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B15" s="3" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="15" ht="14.25" customHeight="1">
-      <c r="A15" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="B15" s="3" t="s">
+      <c r="C15" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="C15" s="2" t="s">
+      <c r="D15" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="D15" s="2" t="s">
+    </row>
+    <row r="16" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A16" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B16" s="3" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="16" ht="14.25" customHeight="1">
-      <c r="A16" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="B16" s="3" t="s">
+      <c r="C16" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="C16" s="2" t="s">
+      <c r="D16" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="D16" s="2" t="s">
+    </row>
+    <row r="17" spans="1:4" ht="14.25" customHeight="1">
+      <c r="A17" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B17" s="3" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="17" ht="14.25" customHeight="1">
-      <c r="A17" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="B17" s="3" t="s">
+      <c r="C17" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="C17" s="2" t="s">
+      <c r="D17" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="D17" s="2" t="s">
+    </row>
+    <row r="18" spans="1:4" ht="14.25" customHeight="1">
+      <c r="A18" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B18" s="3" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="18" ht="14.25" customHeight="1">
-      <c r="A18" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="B18" s="3" t="s">
+      <c r="C18" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="C18" s="2" t="s">
+      <c r="D18" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="D18" s="2" t="s">
+    </row>
+    <row r="19" spans="1:4" ht="14.25" customHeight="1">
+      <c r="A19" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B19" s="3" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="19" ht="14.25" customHeight="1">
-      <c r="A19" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="B19" s="3" t="s">
+      <c r="C19" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="C19" s="2" t="s">
+      <c r="D19" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="D19" s="2" t="s">
+    </row>
+    <row r="20" spans="1:4" ht="14.25" customHeight="1">
+      <c r="A20" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B20" s="3" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="20" ht="14.25" customHeight="1">
-      <c r="A20" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="B20" s="3" t="s">
+      <c r="C20" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="C20" s="2" t="s">
+      <c r="D20" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="D20" s="2" t="s">
+    </row>
+    <row r="21" spans="1:4" ht="14.25" customHeight="1">
+      <c r="A21" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B21" s="3" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="21" ht="14.25" customHeight="1">
-      <c r="A21" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="B21" s="3" t="s">
+      <c r="C21" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="C21" s="2" t="s">
+      <c r="D21" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="D21" s="2" t="s">
+    </row>
+    <row r="22" spans="1:4" ht="14.25" customHeight="1">
+      <c r="A22" s="2" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="22" ht="14.25" customHeight="1">
-      <c r="A22" s="2" t="s">
+      <c r="B22" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="B22" s="3" t="s">
+      <c r="C22" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="C22" s="2" t="s">
+      <c r="D22" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="D22" s="2" t="s">
+    </row>
+    <row r="23" spans="1:4" ht="14.25" customHeight="1">
+      <c r="A23" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B23" s="3" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="23" ht="14.25" customHeight="1">
-      <c r="A23" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="B23" s="3" t="s">
+      <c r="C23" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="C23" s="2" t="s">
+      <c r="D23" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="D23" s="2" t="s">
+    </row>
+    <row r="24" spans="1:4" ht="14.25" customHeight="1">
+      <c r="A24" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B24" s="3" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="24" ht="14.25" customHeight="1">
-      <c r="A24" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="B24" s="3" t="s">
+      <c r="C24" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="C24" s="2" t="s">
+      <c r="D24" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="D24" s="2" t="s">
+    </row>
+    <row r="25" spans="1:4" ht="14.25" customHeight="1">
+      <c r="A25" s="2" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="25" ht="14.25" customHeight="1">
-      <c r="A25" s="2" t="s">
+      <c r="B25" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="B25" s="3" t="s">
+      <c r="C25" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="C25" s="2" t="s">
+      <c r="D25" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="D25" s="2" t="s">
+    </row>
+    <row r="26" spans="1:4" ht="14.25" customHeight="1">
+      <c r="A26" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="B26" s="3" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="26" ht="14.25" customHeight="1">
-      <c r="A26" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="B26" s="3" t="s">
+      <c r="C26" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="C26" s="2" t="s">
+      <c r="D26" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="D26" s="2" t="s">
+    </row>
+    <row r="27" spans="1:4" ht="14.25" customHeight="1">
+      <c r="A27" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="B27" s="3" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="27" ht="14.25" customHeight="1">
-      <c r="A27" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="B27" s="3" t="s">
+      <c r="C27" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="C27" s="2" t="s">
+      <c r="D27" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="D27" s="2" t="s">
+    </row>
+    <row r="28" spans="1:4" ht="14.25" customHeight="1">
+      <c r="A28" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="B28" s="3" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="28" ht="14.25" customHeight="1">
-      <c r="A28" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="B28" s="3" t="s">
+      <c r="C28" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="C28" s="2" t="s">
+      <c r="D28" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="D28" s="2" t="s">
+    </row>
+    <row r="29" spans="1:4" ht="14.25" customHeight="1">
+      <c r="A29" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="B29" s="3" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="29" ht="14.25" customHeight="1">
-      <c r="A29" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="B29" s="3" t="s">
+      <c r="C29" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="C29" s="2" t="s">
+      <c r="D29" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="D29" s="2" t="s">
+    </row>
+    <row r="30" spans="1:4" ht="14.25" customHeight="1">
+      <c r="A30" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="B30" s="3" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="30" ht="14.25" customHeight="1">
-      <c r="A30" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="B30" s="3" t="s">
+      <c r="C30" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="C30" s="2" t="s">
+      <c r="D30" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="D30" s="2" t="s">
+    </row>
+    <row r="31" spans="1:4" ht="14.25" customHeight="1">
+      <c r="A31" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="B31" s="3" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="31" ht="14.25" customHeight="1">
-      <c r="A31" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="B31" s="3" t="s">
+      <c r="C31" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="C31" s="2" t="s">
+      <c r="D31" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="D31" s="2" t="s">
+    </row>
+    <row r="32" spans="1:4" ht="14.25" customHeight="1">
+      <c r="A32" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="B32" s="3" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="32" ht="14.25" customHeight="1">
-      <c r="A32" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="B32" s="3" t="s">
+      <c r="C32" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="C32" s="2" t="s">
+      <c r="D32" s="2" t="s">
         <v>100</v>
-      </c>
-      <c r="D32" s="2" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="33" ht="14.25" customHeight="1"/>
@@ -2032,9 +2058,7 @@
     <row r="999" ht="14.25" customHeight="1"/>
     <row r="1000" ht="14.25" customHeight="1"/>
   </sheetData>
-  <printOptions/>
-  <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Handling variable names in the app
</commit_message>
<xml_diff>
--- a/stream3_visualization/Well-being/data/2025-08-29_EWBI-Renaming of Primary Indicators.xlsx
+++ b/stream3_visualization/Well-being/data/2025-08-29_EWBI-Renaming of Primary Indicators.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\valentin.stuhlfauth\OneDrive - univ-lyon2.fr\Bureau\git-Data4Good\13_democratiser_sobriete\stream3_visualization\Well-being\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="11_E47581067EFA48855B207E265B8E6C1B01B1CEB9" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{FF718A68-91D0-445D-A6A0-B5EEA3E5E72F}"/>
+  <xr:revisionPtr revIDLastSave="6" documentId="11_E47581067EFA48855B207E265B8E6C1B01B1CEB9" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{0402A651-7C8B-46A7-B620-FD51ED567EA0}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8130" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="106">
   <si>
     <t>Current acronym</t>
   </si>
@@ -334,6 +334,15 @@
   </si>
   <si>
     <t>Proposed name</t>
+  </si>
+  <si>
+    <t>HQ-SILC-1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Share of nth decile households living in an over-populated dwelling </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Over-populated dwelling </t>
   </si>
 </sst>
 </file>
@@ -384,11 +393,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -606,8 +616,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A37" sqref="A37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1"/>
@@ -1089,22 +1099,35 @@
         <v>100</v>
       </c>
     </row>
-    <row r="33" ht="14.25" customHeight="1"/>
-    <row r="34" ht="14.25" customHeight="1"/>
-    <row r="35" ht="14.25" customHeight="1"/>
-    <row r="36" ht="14.25" customHeight="1"/>
-    <row r="37" ht="14.25" customHeight="1"/>
-    <row r="38" ht="14.25" customHeight="1"/>
-    <row r="39" ht="14.25" customHeight="1"/>
-    <row r="40" ht="14.25" customHeight="1"/>
-    <row r="41" ht="14.25" customHeight="1"/>
-    <row r="42" ht="14.25" customHeight="1"/>
-    <row r="43" ht="14.25" customHeight="1"/>
-    <row r="44" ht="14.25" customHeight="1"/>
-    <row r="45" ht="14.25" customHeight="1"/>
-    <row r="46" ht="14.25" customHeight="1"/>
-    <row r="47" ht="14.25" customHeight="1"/>
-    <row r="48" ht="14.25" customHeight="1"/>
+    <row r="33" spans="1:4" ht="14.25" customHeight="1">
+      <c r="A33" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B33" t="s">
+        <v>103</v>
+      </c>
+      <c r="C33" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="D33" s="4" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" ht="14.25" customHeight="1"/>
+    <row r="35" spans="1:4" ht="14.25" customHeight="1"/>
+    <row r="36" spans="1:4" ht="14.25" customHeight="1"/>
+    <row r="37" spans="1:4" ht="14.25" customHeight="1"/>
+    <row r="38" spans="1:4" ht="14.25" customHeight="1"/>
+    <row r="39" spans="1:4" ht="14.25" customHeight="1"/>
+    <row r="40" spans="1:4" ht="14.25" customHeight="1"/>
+    <row r="41" spans="1:4" ht="14.25" customHeight="1"/>
+    <row r="42" spans="1:4" ht="14.25" customHeight="1"/>
+    <row r="43" spans="1:4" ht="14.25" customHeight="1"/>
+    <row r="44" spans="1:4" ht="14.25" customHeight="1"/>
+    <row r="45" spans="1:4" ht="14.25" customHeight="1"/>
+    <row r="46" spans="1:4" ht="14.25" customHeight="1"/>
+    <row r="47" spans="1:4" ht="14.25" customHeight="1"/>
+    <row r="48" spans="1:4" ht="14.25" customHeight="1"/>
     <row r="49" ht="14.25" customHeight="1"/>
     <row r="50" ht="14.25" customHeight="1"/>
     <row r="51" ht="14.25" customHeight="1"/>

</xml_diff>